<commit_message>
Adicionando cronograma, e wireframe - illustrator
</commit_message>
<xml_diff>
--- a/Documentos/Cronograma.xlsx
+++ b/Documentos/Cronograma.xlsx
@@ -18,9 +18,83 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="23">
+  <si>
+    <t>Projeto Integrador - Cantinho Fraterno</t>
+  </si>
+  <si>
+    <t>Planejamento</t>
+  </si>
+  <si>
+    <t>Data de entrega</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Briefing</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Card Sorting</t>
+  </si>
+  <si>
+    <t>Personas</t>
+  </si>
+  <si>
+    <t>Wireframe</t>
+  </si>
+  <si>
+    <t>Mapa de navegação</t>
+  </si>
+  <si>
+    <t>Wireframe - Illustrator</t>
+  </si>
+  <si>
+    <t>Modelagem do banco</t>
+  </si>
+  <si>
+    <t>PENDENTE</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>HTML</t>
+  </si>
+  <si>
+    <t>CSS</t>
+  </si>
+  <si>
+    <t>PHP</t>
+  </si>
+  <si>
+    <t>JavaScript</t>
+  </si>
+  <si>
+    <t>Caixa</t>
+  </si>
+  <si>
+    <t>Estoque</t>
+  </si>
+  <si>
+    <t>Cadastro de produtos</t>
+  </si>
+  <si>
+    <t>Relatórios - Doações</t>
+  </si>
+  <si>
+    <t>Relatórios - Financeiro</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,13 +102,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -49,8 +149,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -69,7 +178,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -114,7 +223,7 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -149,7 +258,7 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -331,12 +440,452 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="5" width="18.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="3">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="3">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="3">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="3">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="3">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="3">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="3">
+        <v>43819</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="3">
+        <v>43819</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="3">
+        <v>43819</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="3">
+        <v>43819</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="3">
+        <v>43826</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="3">
+        <v>43826</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="3">
+        <v>43826</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="3">
+        <v>43826</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="3">
+        <v>43833</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="3">
+        <v>43833</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="3">
+        <v>43833</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="3">
+        <v>43833</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="3">
+        <v>43840</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="3">
+        <v>43840</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="3">
+        <v>43840</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" s="3">
+        <v>43840</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37" s="3">
+        <v>43847</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C38" s="3">
+        <v>43847</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" s="3">
+        <v>43847</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>17</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40" s="3">
+        <v>43847</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>14</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C43" s="3">
+        <v>43854</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>15</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C44" s="3">
+        <v>43854</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>16</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45" s="3">
+        <v>43854</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>17</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C46" s="3">
+        <v>43854</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>